<commit_message>
section 6 challenge done
</commit_message>
<xml_diff>
--- a/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
+++ b/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Kuliah Semester 6\Studi Independen\qe_daniel-yogatama-maydiputra\5_Testing Documentation\praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17CB1D9E-6E9B-410A-ABBB-247AC3187329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0753FFE8-359E-4E50-8BA9-315E0DB9B93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6435" windowWidth="29040" windowHeight="15720" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>Login Functionality</t>
   </si>
@@ -172,17 +172,140 @@
     <t>Lupa Password Functionality</t>
   </si>
   <si>
-    <t>Email Valid</t>
-  </si>
-  <si>
     <t>Email INVALID</t>
+  </si>
+  <si>
+    <t>VERIFIKASI bahwa user dapat melakukan navigasi pada semua pilihan produk</t>
+  </si>
+  <si>
+    <t>VERIFIKASI bahwa setiap link menuju ke halaman yang sesuai (produk pulsa apabila di klik menuju ke halaman pulsa)</t>
+  </si>
+  <si>
+    <t>Untuk Kategori Telekomunikasi (Pulsa, Paket Data, Pascabayar, Telkom &amp; Indihome)</t>
+  </si>
+  <si>
+    <t>Untuk BPJS</t>
+  </si>
+  <si>
+    <t>Untuk Listrik PLN</t>
+  </si>
+  <si>
+    <t>ID Pelanggan VALID</t>
+  </si>
+  <si>
+    <t>Email VALID</t>
+  </si>
+  <si>
+    <t>Nomor Handphone VALID</t>
+  </si>
+  <si>
+    <t>Nomor Handphone INVALID</t>
+  </si>
+  <si>
+    <t>Nomor Peserta VALID</t>
+  </si>
+  <si>
+    <t>Nomor Peserta INVALID</t>
+  </si>
+  <si>
+    <t>ID Pelanggan VALID DAN Nomor Handphone VALID</t>
+  </si>
+  <si>
+    <t>ID Pelanggan VALID DAN Nomor Handphone INVALID</t>
+  </si>
+  <si>
+    <t>ID Pelanggan INVALID DAN Nomor Handphone VALID</t>
+  </si>
+  <si>
+    <t>ID Pelanggan INVALID DAN Nomor Handphone INVALID</t>
+  </si>
+  <si>
+    <t>Untuk PDAM</t>
+  </si>
+  <si>
+    <t>Nomor Pelanggan VALID DAN Wilayah VALID</t>
+  </si>
+  <si>
+    <t>Nomor Pelanggan VALID DAN Wilayah INVALID</t>
+  </si>
+  <si>
+    <t>Nomor Pelanggan INVALID DAN Wilayah VALID</t>
+  </si>
+  <si>
+    <t>Nomor Pelanggan INVALID DAN Wilayah INVALID</t>
+  </si>
+  <si>
+    <t>Untuk Internet dan TV Kabel, Bayar Cicilan, Gas, Asuransi</t>
+  </si>
+  <si>
+    <t>ID Pelanggan INVALID</t>
+  </si>
+  <si>
+    <t>Nomor Kartu Kredit VALID</t>
+  </si>
+  <si>
+    <t>Nomor Kartu Kredit INVALID</t>
+  </si>
+  <si>
+    <t>Untuk Kartu Kredit</t>
+  </si>
+  <si>
+    <t>Kota VALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Kota VALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Kota VALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Kota VALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Kota INVALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Kota INVALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Kota INVALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Kota INVALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Form Filling Functionality</t>
+  </si>
+  <si>
+    <t>Untuk PBB</t>
+  </si>
+  <si>
+    <t>Untuk Properti</t>
+  </si>
+  <si>
+    <t>Nama Properti VALID DAN Nomor Pelanggan VALID</t>
+  </si>
+  <si>
+    <t>Nama Properti VALID DAN Nomor Pelanggan INVALID</t>
+  </si>
+  <si>
+    <t>Nama Properti INVALID DAN Nomor Pelanggan VALID</t>
+  </si>
+  <si>
+    <t>Nama Properti INVALID DAN Nomor Pelanggan INVALID</t>
+  </si>
+  <si>
+    <t>Email VALID DAN Nomor Handphone VALID DAN Kredivo</t>
+  </si>
+  <si>
+    <t>Email VALID DAN Nomor Handphone INVALID DAN Kredivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +315,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,22 +346,198 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -542,27 +847,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A4347C-4DF2-43A3-846D-B3D69746BE5D}">
-  <dimension ref="A2:B43"/>
+  <dimension ref="A2:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" customWidth="1"/>
-    <col min="2" max="2" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -629,14 +934,14 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -767,21 +1072,21 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -789,32 +1094,422 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A63:B63"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="A37:B38"/>
+    <mergeCell ref="A43:B43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A34:A35">
+    <cfRule type="duplicateValues" dxfId="16" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:A40 A43">
+    <cfRule type="duplicateValues" dxfId="15" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:A49">
+    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:A45">
+    <cfRule type="duplicateValues" dxfId="12" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:A55">
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:A61 A63">
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:A65">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:A69">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72:A79">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:A85">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88:A91">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
section 7 summary done
</commit_message>
<xml_diff>
--- a/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
+++ b/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Kuliah Semester 6\Studi Independen\qe_daniel-yogatama-maydiputra\5_Testing Documentation\praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0753FFE8-359E-4E50-8BA9-315E0DB9B93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9A3F8E-2657-4451-8F15-4DAD16EAF4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
+    <workbookView xWindow="-4020" yWindow="-14280" windowWidth="17250" windowHeight="8865" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="134">
   <si>
     <t>Login Functionality</t>
   </si>
@@ -73,57 +73,9 @@
     <t>Test Case 9</t>
   </si>
   <si>
-    <t>Nomor Handphone Valid dan Password Valid</t>
-  </si>
-  <si>
-    <t>Nomor Handphone Valid dan Password Invalid</t>
-  </si>
-  <si>
-    <t>Nomor Handphone Invalid dan Password Valid</t>
-  </si>
-  <si>
-    <t>Nomor Handphone Invalid dan Password Invalid</t>
-  </si>
-  <si>
-    <t>Email Valid dan Password Valid</t>
-  </si>
-  <si>
-    <t>Email Valid dan Password Invalid</t>
-  </si>
-  <si>
-    <t>Email Invalid dan Password Valid</t>
-  </si>
-  <si>
-    <t>Email Invalid dan Password Invalid</t>
-  </si>
-  <si>
     <t>Create New Account Functionality (Daftar)</t>
   </si>
   <si>
-    <t>Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone VALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone VALID DAN Password INVALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password INVALID</t>
-  </si>
-  <si>
     <t>Test Case 10</t>
   </si>
   <si>
@@ -145,42 +97,9 @@
     <t>Test Case 16</t>
   </si>
   <si>
-    <t>Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone VALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone VALID DAN Password INVALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password INVALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password VALID</t>
-  </si>
-  <si>
-    <t>Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
-  </si>
-  <si>
     <t>Lupa Password Functionality</t>
   </si>
   <si>
-    <t>Email INVALID</t>
-  </si>
-  <si>
-    <t>VERIFIKASI bahwa user dapat melakukan navigasi pada semua pilihan produk</t>
-  </si>
-  <si>
-    <t>VERIFIKASI bahwa setiap link menuju ke halaman yang sesuai (produk pulsa apabila di klik menuju ke halaman pulsa)</t>
-  </si>
-  <si>
     <t>Untuk Kategori Telekomunikasi (Pulsa, Paket Data, Pascabayar, Telkom &amp; Indihome)</t>
   </si>
   <si>
@@ -193,9 +112,6 @@
     <t>ID Pelanggan VALID</t>
   </si>
   <si>
-    <t>Email VALID</t>
-  </si>
-  <si>
     <t>Nomor Handphone VALID</t>
   </si>
   <si>
@@ -299,6 +215,228 @@
   </si>
   <si>
     <t>Email VALID DAN Nomor Handphone INVALID DAN Kredivo</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone Valid dan Password Valid</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone Valid dan Password Invalid</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone Invalid dan Password Valid</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone Invalid dan Password Invalid</t>
+  </si>
+  <si>
+    <t>Enter Email Valid dan Password Valid</t>
+  </si>
+  <si>
+    <t>Enter Email Valid dan Password Invalid</t>
+  </si>
+  <si>
+    <t>Enter Email Invalid dan Password Valid</t>
+  </si>
+  <si>
+    <t>Enter Email Invalid dan Password Invalid</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone VALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone VALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap VALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone VALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone VALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email VALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone VALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Lengkap INVALID DAN Email INVALID DAN Nomor Handphone INVALID DAN Password INVALID</t>
+  </si>
+  <si>
+    <t>Enter Email VALID</t>
+  </si>
+  <si>
+    <t>Enter Email INVALID</t>
+  </si>
+  <si>
+    <t>Press Pulsa</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Press Paket Data</t>
+  </si>
+  <si>
+    <t>Press Pasca Bayar</t>
+  </si>
+  <si>
+    <t>Press Telkom &amp; Indihome</t>
+  </si>
+  <si>
+    <t>Press BPJS Ketenagakerjaan</t>
+  </si>
+  <si>
+    <t>Press Listrik PLN</t>
+  </si>
+  <si>
+    <t>Press PDAM</t>
+  </si>
+  <si>
+    <t>Press Internet dan TV Kabel</t>
+  </si>
+  <si>
+    <t>Press BPJS Kesehatan</t>
+  </si>
+  <si>
+    <t>Press Bayar Cicilan</t>
+  </si>
+  <si>
+    <t>Press Kartu Kredit</t>
+  </si>
+  <si>
+    <t>Press PBB</t>
+  </si>
+  <si>
+    <t>Press Gas</t>
+  </si>
+  <si>
+    <t>Press Properti</t>
+  </si>
+  <si>
+    <t>Press Asuransi</t>
+  </si>
+  <si>
+    <t>Press Voucher Game</t>
+  </si>
+  <si>
+    <t>Press Voucher Deals</t>
+  </si>
+  <si>
+    <t>Press Voucher Edukasi</t>
+  </si>
+  <si>
+    <t>Press Voucher Streaming</t>
+  </si>
+  <si>
+    <t>Press Uang Elektronik</t>
+  </si>
+  <si>
+    <t>Press Sepulsa Berkah</t>
+  </si>
+  <si>
+    <t>Test Case 17</t>
+  </si>
+  <si>
+    <t>Test Case 18</t>
+  </si>
+  <si>
+    <t>Test Case 19</t>
+  </si>
+  <si>
+    <t>Test Case 20</t>
+  </si>
+  <si>
+    <t>Test Case 21</t>
+  </si>
+  <si>
+    <t>Page Pulsa</t>
+  </si>
+  <si>
+    <t>Page Paket Data</t>
+  </si>
+  <si>
+    <t>Page Pasca Bayar</t>
+  </si>
+  <si>
+    <t>PageTelkom &amp; Indihome</t>
+  </si>
+  <si>
+    <t>Page BPJS Ketenagakerjaan</t>
+  </si>
+  <si>
+    <t>Page Listrik PLN</t>
+  </si>
+  <si>
+    <t>Page PDAM</t>
+  </si>
+  <si>
+    <t>Page Internet dan TV Kabel</t>
+  </si>
+  <si>
+    <t>Page BPJS Kesehatan</t>
+  </si>
+  <si>
+    <t>Page Bayar Cicilan</t>
+  </si>
+  <si>
+    <t>Page Kartu Kredit</t>
+  </si>
+  <si>
+    <t>Page PBB</t>
+  </si>
+  <si>
+    <t>Page Gas</t>
+  </si>
+  <si>
+    <t>Page Properti</t>
+  </si>
+  <si>
+    <t>Page Asuransi</t>
+  </si>
+  <si>
+    <t>Page Voucher Game</t>
+  </si>
+  <si>
+    <t>Page Voucher Deals</t>
+  </si>
+  <si>
+    <t>Page Voucher Edukasi</t>
+  </si>
+  <si>
+    <t>Page Voucher Streaming</t>
+  </si>
+  <si>
+    <t>Page Uang Elektronik</t>
+  </si>
+  <si>
+    <t>Page Sepulsa Berkah</t>
   </si>
 </sst>
 </file>
@@ -348,20 +486,20 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,34 +985,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A4347C-4DF2-43A3-846D-B3D69746BE5D}">
-  <dimension ref="A2:B91"/>
+  <dimension ref="A2:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" customWidth="1"/>
     <col min="2" max="2" width="98.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -882,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -890,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -898,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -906,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -914,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -922,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,25 +1067,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -956,7 +1093,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -964,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -972,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -980,7 +1117,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -988,7 +1125,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -996,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1004,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1012,503 +1149,721 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="B39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-    </row>
-    <row r="42" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="4"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="4"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B63" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="B64" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>3</v>
       </c>
-      <c r="B48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="3"/>
+      <c r="B67" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>3</v>
       </c>
-      <c r="B68" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" s="3"/>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" t="s">
-        <v>75</v>
-      </c>
+      <c r="A76" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
-        <v>82</v>
-      </c>
+      <c r="A82" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" t="s">
-        <v>85</v>
-      </c>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="3"/>
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>4</v>
-      </c>
-      <c r="B89" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>5</v>
-      </c>
+      <c r="A90" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="3"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A63:B63"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="A37:B38"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A34:A35">
     <cfRule type="duplicateValues" dxfId="16" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A40 A43">
-    <cfRule type="duplicateValues" dxfId="15" priority="21"/>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
+  <conditionalFormatting sqref="A67:A68">
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:A49">
-    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
+  <conditionalFormatting sqref="A63:A64">
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44:A45">
-    <cfRule type="duplicateValues" dxfId="12" priority="15"/>
+  <conditionalFormatting sqref="A71:A74">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52:A55">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+  <conditionalFormatting sqref="A77:A80 A82">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58:A61 A63">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  <conditionalFormatting sqref="A83:A84">
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A64:A65">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="A87:A88">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A68:A69">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="A91:A98">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72:A79">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="A101:A104">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A82:A85">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="A107:A110">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A88:A91">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A62 A39:A59">
+    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Section 5 challenge done, Section 7 Challenge done
</commit_message>
<xml_diff>
--- a/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
+++ b/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Kuliah Semester 6\Studi Independen\qe_daniel-yogatama-maydiputra\5_Testing Documentation\praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9A3F8E-2657-4451-8F15-4DAD16EAF4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64307F3-B301-4794-B1B0-27815A5B403F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4020" yWindow="-14280" windowWidth="17250" windowHeight="8865" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="136">
   <si>
     <t>Login Functionality</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Choose Product Functionality</t>
   </si>
   <si>
-    <t>Payment Method Functionality</t>
-  </si>
-  <si>
     <t>Test Case 1</t>
   </si>
   <si>
@@ -109,87 +106,15 @@
     <t>Untuk Listrik PLN</t>
   </si>
   <si>
-    <t>ID Pelanggan VALID</t>
-  </si>
-  <si>
-    <t>Nomor Handphone VALID</t>
-  </si>
-  <si>
-    <t>Nomor Handphone INVALID</t>
-  </si>
-  <si>
-    <t>Nomor Peserta VALID</t>
-  </si>
-  <si>
-    <t>Nomor Peserta INVALID</t>
-  </si>
-  <si>
-    <t>ID Pelanggan VALID DAN Nomor Handphone VALID</t>
-  </si>
-  <si>
-    <t>ID Pelanggan VALID DAN Nomor Handphone INVALID</t>
-  </si>
-  <si>
-    <t>ID Pelanggan INVALID DAN Nomor Handphone VALID</t>
-  </si>
-  <si>
-    <t>ID Pelanggan INVALID DAN Nomor Handphone INVALID</t>
-  </si>
-  <si>
     <t>Untuk PDAM</t>
   </si>
   <si>
-    <t>Nomor Pelanggan VALID DAN Wilayah VALID</t>
-  </si>
-  <si>
-    <t>Nomor Pelanggan VALID DAN Wilayah INVALID</t>
-  </si>
-  <si>
-    <t>Nomor Pelanggan INVALID DAN Wilayah VALID</t>
-  </si>
-  <si>
-    <t>Nomor Pelanggan INVALID DAN Wilayah INVALID</t>
-  </si>
-  <si>
     <t>Untuk Internet dan TV Kabel, Bayar Cicilan, Gas, Asuransi</t>
   </si>
   <si>
-    <t>ID Pelanggan INVALID</t>
-  </si>
-  <si>
-    <t>Nomor Kartu Kredit VALID</t>
-  </si>
-  <si>
-    <t>Nomor Kartu Kredit INVALID</t>
-  </si>
-  <si>
     <t>Untuk Kartu Kredit</t>
   </si>
   <si>
-    <t>Kota VALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak VALID</t>
-  </si>
-  <si>
-    <t>Kota VALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak INVALID</t>
-  </si>
-  <si>
-    <t>Kota VALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak VALID</t>
-  </si>
-  <si>
-    <t>Kota VALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak INVALID</t>
-  </si>
-  <si>
-    <t>Kota INVALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak VALID</t>
-  </si>
-  <si>
-    <t>Kota INVALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak INVALID</t>
-  </si>
-  <si>
-    <t>Kota INVALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak VALID</t>
-  </si>
-  <si>
-    <t>Kota INVALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak INVALID</t>
-  </si>
-  <si>
     <t>Form Filling Functionality</t>
   </si>
   <si>
@@ -199,24 +124,6 @@
     <t>Untuk Properti</t>
   </si>
   <si>
-    <t>Nama Properti VALID DAN Nomor Pelanggan VALID</t>
-  </si>
-  <si>
-    <t>Nama Properti VALID DAN Nomor Pelanggan INVALID</t>
-  </si>
-  <si>
-    <t>Nama Properti INVALID DAN Nomor Pelanggan VALID</t>
-  </si>
-  <si>
-    <t>Nama Properti INVALID DAN Nomor Pelanggan INVALID</t>
-  </si>
-  <si>
-    <t>Email VALID DAN Nomor Handphone VALID DAN Kredivo</t>
-  </si>
-  <si>
-    <t>Email VALID DAN Nomor Handphone INVALID DAN Kredivo</t>
-  </si>
-  <si>
     <t>Enter Nomor Handphone Valid dan Password Valid</t>
   </si>
   <si>
@@ -437,6 +344,105 @@
   </si>
   <si>
     <t>Page Sepulsa Berkah</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone VALID DAN Kredivo</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone VALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Peserta VALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Peserta INVALID</t>
+  </si>
+  <si>
+    <t>Enter ID Pelanggan VALID DAN Nomor Handphone VALID</t>
+  </si>
+  <si>
+    <t>Enter ID Pelanggan VALID DAN Nomor Handphone INVALID</t>
+  </si>
+  <si>
+    <t>Enter ID Pelanggan INVALID DAN Nomor Handphone VALID</t>
+  </si>
+  <si>
+    <t>Enter ID Pelanggan INVALID DAN Nomor Handphone INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Pelanggan VALID DAN Wilayah VALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Pelanggan VALID DAN Wilayah INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Pelanggan INVALID DAN Wilayah VALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Pelanggan INVALID DAN Wilayah INVALID</t>
+  </si>
+  <si>
+    <t>Enter ID Pelanggan VALID</t>
+  </si>
+  <si>
+    <t>Enter ID Pelanggan INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Kartu Kredit VALID</t>
+  </si>
+  <si>
+    <t>Enter Nomor Kartu Kredit INVALID</t>
+  </si>
+  <si>
+    <t>Enter Kota VALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Enter Kota VALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Enter Kota VALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Enter Kota VALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Enter Kota INVALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Enter Kota INVALID DAN Tahun Pajak VALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Enter Kota INVALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak VALID</t>
+  </si>
+  <si>
+    <t>Enter Kota INVALID DAN Tahun Pajak INVALID DAN Nomor Objek Pajak INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Properti VALID DAN Nomor Pelanggan VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Properti VALID DAN Nomor Pelanggan INVALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Properti INVALID DAN Nomor Pelanggan VALID</t>
+  </si>
+  <si>
+    <t>Enter Nama Properti INVALID DAN Nomor Pelanggan INVALID</t>
+  </si>
+  <si>
+    <t>Buy Pulsa Payment Method Functionality</t>
+  </si>
+  <si>
+    <t>Enter Nomor Handphone INVALID DAN Kredivo</t>
+  </si>
+  <si>
+    <t>Email Nomor Handphone VALID DAN Gopay</t>
+  </si>
+  <si>
+    <t>Email Nomor Handphone INVALID DAN Gopay</t>
   </si>
 </sst>
 </file>
@@ -489,16 +495,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,7 +993,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A4347C-4DF2-43A3-846D-B3D69746BE5D}">
   <dimension ref="A2:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -997,485 +1005,485 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5"/>
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1483,31 +1491,31 @@
       <c r="B60" s="1"/>
     </row>
     <row r="61" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B61" s="4"/>
+      <c r="A61" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" s="4"/>
+      <c r="A62" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1515,294 +1523,295 @@
       <c r="B65" s="1"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="3"/>
+      <c r="A66" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="3"/>
+      <c r="A70" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B76" s="3"/>
+      <c r="A76" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B82" s="3"/>
+      <c r="A82" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B86" s="3"/>
+      <c r="A86" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B90" s="3"/>
+      <c r="A90" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B100" s="3"/>
+      <c r="A100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B100" s="5"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B104" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="3"/>
+      <c r="A106" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B106" s="5"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B109" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A13:B14"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="A90:B90"/>
@@ -1812,6 +1821,11 @@
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A76:B76"/>
     <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="A62:B62"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A34:A35">

</xml_diff>

<commit_message>
Section 5 Challenge done
</commit_message>
<xml_diff>
--- a/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
+++ b/5_Testing Documentation/praktikum/TestScenario_sepulsacom.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Kuliah Semester 6\Studi Independen\qe_daniel-yogatama-maydiputra\5_Testing Documentation\praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D012121E-B11A-49B0-8E0D-ABDF1E9E4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DD605-4785-4E71-BD18-1CF69F4A5DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70C96A93-F658-4333-8A96-74E5D445B7E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="151">
   <si>
     <t>Login Functionality</t>
   </si>
@@ -479,6 +480,15 @@
   </si>
   <si>
     <t>Precondition</t>
+  </si>
+  <si>
+    <t>Succesfully Pay with Kredivo</t>
+  </si>
+  <si>
+    <t>Succesfully Pay with Gopay</t>
+  </si>
+  <si>
+    <t>Payment Can't be done</t>
   </si>
 </sst>
 </file>
@@ -533,16 +543,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A4347C-4DF2-43A3-846D-B3D69746BE5D}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116:C125"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,10 +1302,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -1761,8 +1771,8 @@
       <c r="C82" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -2188,7 +2198,7 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B132" s="7" t="s">
+      <c r="B132" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2216,6 +2226,9 @@
       <c r="B134" t="s">
         <v>74</v>
       </c>
+      <c r="C134" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
@@ -2224,6 +2237,9 @@
       <c r="B135" t="s">
         <v>104</v>
       </c>
+      <c r="C135" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
@@ -2232,6 +2248,9 @@
       <c r="B136" t="s">
         <v>105</v>
       </c>
+      <c r="C136" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
@@ -2239,6 +2258,9 @@
       </c>
       <c r="B137" t="s">
         <v>106</v>
+      </c>
+      <c r="C137" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2269,4 +2291,16 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3C6AC0-94CB-40A9-92A9-5C607BB8942F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>